<commit_message>
updated men's awards data
</commit_message>
<xml_diff>
--- a/Awards/Men/Track & Field (Indoor).xlsx
+++ b/Awards/Men/Track & Field (Indoor).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dengjiahao\Desktop\Athlete\Awards\Men\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBF9BBF-55CB-4F61-BD5C-798C9228F4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611CCFE4-8569-4622-B041-6FE2D3842C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="612" windowWidth="17280" windowHeight="10008" xr2:uid="{9C3D1E80-FFC7-49B5-A22D-BD7D30B75EB4}"/>
+    <workbookView xWindow="-620" yWindow="780" windowWidth="18660" windowHeight="8630" xr2:uid="{9C3D1E80-FFC7-49B5-A22D-BD7D30B75EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="3" r:id="rId1"/>
@@ -449,17 +449,17 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -487,7 +487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -501,7 +501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -515,7 +515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2010</v>
       </c>
@@ -529,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2009</v>
       </c>

</xml_diff>